<commit_message>
atualização da base e do histórico
</commit_message>
<xml_diff>
--- a/data/historico_cestas_mutiroes.xlsx
+++ b/data/historico_cestas_mutiroes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A62FB4E-C2D3-4A70-BDC0-736085DE0D2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D86B68-E19F-420B-AD52-6CB827BF3ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4860" yWindow="9135" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cestas" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>alface crespa</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>corte de bambus para utilização no novo canteiro de tomate/vagem</t>
+  </si>
+  <si>
+    <t>rúcula</t>
+  </si>
+  <si>
+    <t>manjericão</t>
+  </si>
+  <si>
+    <t>azedinha</t>
+  </si>
+  <si>
+    <t>inhame</t>
+  </si>
+  <si>
+    <t>jiló</t>
+  </si>
+  <si>
+    <t>salsão</t>
   </si>
 </sst>
 </file>
@@ -392,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +492,94 @@
       </c>
       <c r="B9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44352</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>